<commit_message>
Completed Verification of Zhihing Inheritance Work
</commit_message>
<xml_diff>
--- a/Project_Inheritance_Documentation/Branch_2_ Inheritance/Zhihong_Deng_Handover.xlsx
+++ b/Project_Inheritance_Documentation/Branch_2_ Inheritance/Zhihong_Deng_Handover.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f337a85aa8871bf9/Desktop/japanese_project/japanese-handwriting-analysis/Project_Inheritance_Documentation/Branch_2_ Inheritance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANU\Semester_3\Advanced_Computing_Project\Project_Repo\japanese-handwriting-analysis\Project_Inheritance_Documentation\Branch_2_ Inheritance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{140B3B82-FA32-4F43-B43B-0F7D960488D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49DED262-38A7-407A-9936-71918C37ACAC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293E5EB4-DB39-424A-8A92-718C07CAA547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="62">
   <si>
     <t>To be filled by continuing member who is handing over</t>
   </si>
@@ -200,7 +200,25 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>Zhihong Deng</t>
+    <t>Muhammad Arslan</t>
+  </si>
+  <si>
+    <t>Yes, Zhihong told me about this task</t>
+  </si>
+  <si>
+    <t>Yeah, he highlighted these things to me in repo and gave me a bit overview but I haven't ran it on my system yet, but some modules did worked on my laptop</t>
+  </si>
+  <si>
+    <t>Can explain it to the new members next semester and we can try to improve it and make it more better in working.</t>
+  </si>
+  <si>
+    <t>Yes, Zhihong told me about this task and I understood this part as well</t>
+  </si>
+  <si>
+    <t>Yes, I have understood this part and but need to further test it on my system to get better idea of it</t>
+  </si>
+  <si>
+    <t>Will need to put some effort in to digest this work and will try to incorporate all the knowledge base I have regarding this issue it to the new members as well</t>
   </si>
 </sst>
 </file>
@@ -405,6 +423,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -423,7 +442,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -702,48 +720,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="6.3984375" customWidth="1"/>
-    <col min="3" max="3" width="41.265625" customWidth="1"/>
-    <col min="4" max="4" width="17.1328125" customWidth="1"/>
-    <col min="5" max="5" width="16.265625" customWidth="1"/>
-    <col min="6" max="6" width="33.1328125" customWidth="1"/>
-    <col min="7" max="7" width="21.265625" customWidth="1"/>
-    <col min="8" max="10" width="21.46484375" customWidth="1"/>
-    <col min="11" max="11" width="20.3984375" customWidth="1"/>
-    <col min="12" max="12" width="38.86328125" customWidth="1"/>
-    <col min="13" max="14" width="21.46484375" customWidth="1"/>
+    <col min="1" max="2" width="6.42578125" customWidth="1"/>
+    <col min="3" max="3" width="41.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="8" max="10" width="21.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1"/>
+    <col min="12" max="12" width="38.85546875" customWidth="1"/>
+    <col min="13" max="13" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" customWidth="1"/>
     <col min="15" max="15" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="16" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="17"/>
-      <c r="O1" s="18"/>
-    </row>
-    <row r="2" spans="1:15" ht="28.5">
+      <c r="N1" s="18"/>
+      <c r="O1" s="19"/>
+    </row>
+    <row r="2" spans="1:15" ht="30">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -821,7 +840,7 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:15" ht="85.5">
+    <row r="4" spans="1:15" ht="120">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -847,7 +866,7 @@
       <c r="I4" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="13">
         <v>45569</v>
       </c>
       <c r="K4" s="6" t="s">
@@ -856,11 +875,17 @@
       <c r="L4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-    </row>
-    <row r="5" spans="1:15" ht="80.099999999999994" customHeight="1">
+      <c r="M4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="138.75" customHeight="1">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -886,7 +911,7 @@
       <c r="I5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="13">
         <v>45569</v>
       </c>
       <c r="K5" s="7" t="s">
@@ -895,11 +920,17 @@
       <c r="L5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-    </row>
-    <row r="6" spans="1:15" ht="85.5">
+      <c r="M5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="138.75" customHeight="1">
       <c r="A6" s="4">
         <v>3</v>
       </c>
@@ -925,7 +956,7 @@
       <c r="I6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="13">
         <v>45569</v>
       </c>
       <c r="K6" s="6" t="s">
@@ -934,11 +965,17 @@
       <c r="L6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-    </row>
-    <row r="7" spans="1:15" ht="92.1" customHeight="1">
+      <c r="M6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="126" customHeight="1">
       <c r="A7" s="4">
         <v>4</v>
       </c>
@@ -964,7 +1001,7 @@
       <c r="I7" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="13">
         <v>45569</v>
       </c>
       <c r="K7" s="6" t="s">
@@ -973,11 +1010,17 @@
       <c r="L7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-    </row>
-    <row r="8" spans="1:15" ht="85.5">
+      <c r="M7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="120">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -1003,7 +1046,7 @@
       <c r="I8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="13">
         <v>45569</v>
       </c>
       <c r="K8" s="6" t="s">
@@ -1012,9 +1055,15 @@
       <c r="L8" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
+      <c r="M8" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="9" spans="1:15" ht="127.5" customHeight="1">
       <c r="A9" s="4">
@@ -1042,7 +1091,7 @@
       <c r="I9" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="13">
         <v>45569</v>
       </c>
       <c r="K9" s="6" t="s">
@@ -1051,9 +1100,15 @@
       <c r="L9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
+      <c r="M9" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="10" spans="1:15" ht="124.5" customHeight="1">
       <c r="A10" s="4">
@@ -1081,7 +1136,7 @@
       <c r="I10" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="13">
         <v>45569</v>
       </c>
       <c r="K10" s="6" t="s">
@@ -1090,9 +1145,15 @@
       <c r="L10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
+      <c r="M10" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="11" spans="1:15" ht="105.95" customHeight="1">
       <c r="A11" s="4">
@@ -1120,7 +1181,7 @@
       <c r="I11" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="13">
         <v>45569</v>
       </c>
       <c r="K11" s="6" t="s">
@@ -1129,9 +1190,15 @@
       <c r="L11" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
+      <c r="M11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="12" spans="1:15" s="1" customFormat="1" ht="106.5" customHeight="1">
       <c r="A12" s="5">
@@ -1159,7 +1226,7 @@
       <c r="I12" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="13">
         <v>45569</v>
       </c>
       <c r="K12" s="6" t="s">
@@ -1168,9 +1235,15 @@
       <c r="L12" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
+      <c r="M12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="4"/>

</xml_diff>